<commit_message>
Updated script for proteins to include LC3
</commit_message>
<xml_diff>
--- a/scripts/MitoProteinAnalysis/PostReviewMitoWesterns.xlsx
+++ b/scripts/MitoProteinAnalysis/PostReviewMitoWesterns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Stephenson\Mouse Work\Maternal MCP230 exposure\Western blots\Quads\Post review blots\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esteph16\Documents\GitHub\ObesityParticulateTreatment\scripts\MitoProteinAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>NDUFB8</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>SLN</t>
+  </si>
+  <si>
+    <t>LC3</t>
   </si>
 </sst>
 </file>
@@ -374,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="G27" sqref="G26:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -410,8 +413,11 @@
       <c r="I1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>276</v>
       </c>
@@ -439,8 +445,11 @@
       <c r="I2">
         <v>0.43976474573583102</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0.67591751391550914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>277</v>
       </c>
@@ -468,8 +477,11 @@
       <c r="I3">
         <v>0.4039177700424238</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>1.5836664465981622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>278</v>
       </c>
@@ -497,8 +509,11 @@
       <c r="I4">
         <v>1.1265785295055808</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>1.4478299833717341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>279</v>
       </c>
@@ -526,8 +541,11 @@
       <c r="I5">
         <v>1.4567495204272489</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>1.1400664926442372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>280</v>
       </c>
@@ -555,8 +573,11 @@
       <c r="I6">
         <v>1.5729894342889159</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0.8885862538532423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>281</v>
       </c>
@@ -581,8 +602,11 @@
       <c r="H7">
         <v>0.76653180222738315</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0.90842775062572723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>290</v>
       </c>
@@ -610,8 +634,11 @@
       <c r="I8">
         <v>0.57369757586764669</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1.0621257672209483</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>291</v>
       </c>
@@ -639,8 +666,11 @@
       <c r="I9">
         <v>1.0604473023786718</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>0.61341074018439312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>292</v>
       </c>
@@ -668,8 +698,11 @@
       <c r="I10">
         <v>1.7238787383873213</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>0.39080052503290935</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>293</v>
       </c>
@@ -697,8 +730,11 @@
       <c r="I11">
         <v>0.64197638336635954</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>0.82817440272029752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>201</v>
       </c>
@@ -726,8 +762,11 @@
       <c r="I12">
         <v>0.34245232816823429</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>1.0004217638625819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>202</v>
       </c>
@@ -755,8 +794,11 @@
       <c r="I13">
         <v>0.5512732208312906</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>0.91894361822272796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>203</v>
       </c>
@@ -784,8 +826,11 @@
       <c r="I14">
         <v>2.7937192411456748</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>1.0888062312362772</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>204</v>
       </c>
@@ -813,8 +858,11 @@
       <c r="I15">
         <v>2.5572209023274066</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>1.3329024372005578</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>207</v>
       </c>
@@ -842,8 +890,11 @@
       <c r="I16">
         <v>1.2215606663616907</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>1.3021098280795838</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>208</v>
       </c>
@@ -871,8 +922,11 @@
       <c r="I17">
         <v>0.60611960391135367</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>0.8718845568381417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>209</v>
       </c>
@@ -900,8 +954,11 @@
       <c r="I18">
         <v>1.1927796215804063</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>1.0410002113096071</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>214</v>
       </c>
@@ -929,8 +986,11 @@
       <c r="I19">
         <v>1.422975280265582</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>1.1031072281693164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>250</v>
       </c>
@@ -958,8 +1018,11 @@
       <c r="I20">
         <v>1.1447176216445916</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>0.81031859699962649</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2500</v>
       </c>
@@ -986,6 +1049,9 @@
       </c>
       <c r="I21">
         <v>0.60384917063911503</v>
+      </c>
+      <c r="J21">
+        <v>0.93605589873058992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>